<commit_message>
add and wire up InitAllApplications
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.coker\Documents\UiPath\UiPathMockPOC-ZipCodeLookup\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE7AD7-49D1-4EE9-A198-CC04842EF34E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -159,14 +156,35 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>ZipCodeLookup</t>
+  </si>
+  <si>
+    <t>UiPathMockPOC-ZipCodeLookup</t>
+  </si>
+  <si>
+    <t>Excel_ZipCodesDir</t>
+  </si>
+  <si>
+    <t>C:\Users\james.coker\Documents\UiPath\UiPathMockPOC-ZipCodeLookup\Data</t>
+  </si>
+  <si>
+    <t>Excel_LocationsFilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\james.coker\Documents\UiPath\UiPathMockPOC-ZipCodeLookup\Locations\Locations.xlsx</t>
+  </si>
+  <si>
+    <t>USPS_URL</t>
+  </si>
+  <si>
+    <t>https://tools.usps.com/go/ZipLookupAction!input.action</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +208,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,10 +233,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,8 +247,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,7 +568,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -585,22 +615,22 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -609,15 +639,36 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1610,8 +1661,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{BBF61411-8ACC-4738-A41B-36FA25BAB118}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1673,18 +1727,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1762,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1795,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1806,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2802,7 +2856,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Invoke and wire up Process workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.coker\Documents\UiPath\UiPathMockPOC-ZipCodeLookup\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE7AD7-49D1-4EE9-A198-CC04842EF34E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B229AA45-22B5-4827-86CB-983B4530BE58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,89 +95,88 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>ZipCodeLookup</t>
+  </si>
+  <si>
+    <t>UiPathMockPOC-ZipCodeLookup</t>
+  </si>
+  <si>
+    <t>Excel_ZipCodesDir</t>
+  </si>
+  <si>
+    <t>C:\Users\james.coker\Documents\UiPath\UiPathMockPOC-ZipCodeLookup\Data</t>
+  </si>
+  <si>
+    <t>Excel_LocationsFilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\james.coker\Documents\UiPath\UiPathMockPOC-ZipCodeLookup\Locations\Locations.xlsx</t>
+  </si>
+  <si>
+    <t>USPS_URL</t>
+  </si>
+  <si>
+    <t>https://tools.usps.com/go/ZipLookupAction!input.action</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ZipCodeLookup</t>
-  </si>
-  <si>
-    <t>UiPathMockPOC-ZipCodeLookup</t>
-  </si>
-  <si>
-    <t>Excel_ZipCodesDir</t>
-  </si>
-  <si>
-    <t>C:\Users\james.coker\Documents\UiPath\UiPathMockPOC-ZipCodeLookup\Data</t>
-  </si>
-  <si>
-    <t>Excel_LocationsFilePath</t>
-  </si>
-  <si>
-    <t>C:\Users\james.coker\Documents\UiPath\UiPathMockPOC-ZipCodeLookup\Locations\Locations.xlsx</t>
-  </si>
-  <si>
-    <t>USPS_URL</t>
-  </si>
-  <si>
-    <t>https://tools.usps.com/go/ZipLookupAction!input.action</t>
   </si>
 </sst>
 </file>
@@ -568,7 +567,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -615,10 +614,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -626,11 +625,11 @@
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -639,7 +638,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -647,26 +646,26 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1727,18 +1726,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1762,7 +1761,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1784,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1795,7 +1794,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1806,53 +1805,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2856,7 +2855,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>